<commit_message>
cambio inicio de sesion
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Usuario2.xlsx
+++ b/src/test/resources/data/Usuario2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PARDOC\Desktop\SaldoLineas\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\38513959\Downloads\SaldoLineas\SaldoLineas\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A31B2A-CAB2-4DF1-B601-B5A2067EA1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Usuario</t>
   </si>
@@ -27,23 +28,20 @@
     <t>Contrasena</t>
   </si>
   <si>
-    <t>45111410</t>
-  </si>
-  <si>
-    <t>nef18@*ALE</t>
-  </si>
-  <si>
     <t>Numero</t>
   </si>
   <si>
-    <t>3213270592</t>
+    <t>lorena.rodriguez@claro.com.co</t>
+  </si>
+  <si>
+    <t>Pruebas2026*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +53,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,19 +98,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -121,9 +129,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -161,9 +169,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,7 +206,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,7 +241,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -406,11 +414,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,35 +429,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BE7C5FAA-903B-4DDA-BBE8-CA1CA52C6E37}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;6&amp;K000000 Clasificación: Uso Interno. Documento Claro Colombia</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>